<commit_message>
add templates and targets
</commit_message>
<xml_diff>
--- a/configs/global_config.xlsx
+++ b/configs/global_config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>SLURM_iteration</t>
   </si>
@@ -28,40 +28,34 @@
     <t>material</t>
   </si>
   <si>
-    <t>hardeningLaw</t>
-  </si>
-  <si>
-    <t>geometry</t>
-  </si>
-  <si>
-    <t>curveIndex</t>
-  </si>
-  <si>
-    <t>deviationPercent</t>
+    <t>CPLaw</t>
+  </si>
+  <si>
+    <t>grains</t>
+  </si>
+  <si>
+    <t>strainRates</t>
   </si>
   <si>
     <t>optimizerName</t>
   </si>
   <si>
-    <t>yieldingIndex</t>
-  </si>
-  <si>
     <t>one_node_small</t>
   </si>
   <si>
-    <t>DP1000_25C</t>
-  </si>
-  <si>
-    <t>SwiftVoce</t>
-  </si>
-  <si>
-    <t>NDBR50,NDBR20,NDBR6,CHD6,SH</t>
-  </si>
-  <si>
-    <t>BOTORCH</t>
-  </si>
-  <si>
-    <t>700;800;800;800;500</t>
+    <t>ferrite</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>1441;2744;3198</t>
+  </si>
+  <si>
+    <t>0.1;1;100</t>
+  </si>
+  <si>
+    <t>LinearRegression</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -70,37 +64,16 @@
     <t>one_node_test</t>
   </si>
   <si>
-    <t>Swift</t>
-  </si>
-  <si>
-    <t>By convention, curveIndex 1 corresponds to experimental target curves</t>
-  </si>
-  <si>
-    <t>BO</t>
-  </si>
-  <si>
-    <t>DP1000_400C</t>
-  </si>
-  <si>
-    <t>NDBR50,NDBR6,CHD6</t>
-  </si>
-  <si>
-    <t>curveIndex larger than 1 are simulated target curves</t>
-  </si>
-  <si>
-    <t>200;200;1200</t>
+    <t/>
+  </si>
+  <si>
+    <t>martensite</t>
+  </si>
+  <si>
+    <t>DB</t>
   </si>
   <si>
     <t>two_nodes_small</t>
-  </si>
-  <si>
-    <t>QP1000_25C</t>
-  </si>
-  <si>
-    <t>NDBR25,NDBR6,CHD6</t>
-  </si>
-  <si>
-    <t>220;260;280</t>
   </si>
   <si>
     <t>one_node_test if you dont want to queue. However, time limit is 15 minutes so simulations will sometimes fail due to timeout</t>
@@ -159,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -180,6 +153,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -499,28 +478,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="32.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="32.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="11" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="12" width="27.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="10" width="32.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="10" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="14" width="17.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="38.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="14" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="14" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33" customFormat="1" s="1">
@@ -539,65 +514,49 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="6">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="C2" s="6">
         <v>10000</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="6">
-        <v>1</v>
-      </c>
-      <c r="H2" s="6">
-        <v>2</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="5"/>
@@ -607,119 +566,77 @@
       <c r="E3" s="7"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="6"/>
+      <c r="H3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="D6" s="7"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="5"/>
@@ -727,257 +644,201 @@
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="5"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="8"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="5"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="8"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="5"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="8"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="8"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="5"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="8"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="8"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="5"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="8"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="5"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="8"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="8"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="5"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="8"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="8"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="5"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
-      <c r="F18" s="8"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="8"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="5"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
-      <c r="F19" s="8"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="8"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="5"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish adding templates and targets
</commit_message>
<xml_diff>
--- a/configs/global_config.xlsx
+++ b/configs/global_config.xlsx
@@ -43,7 +43,7 @@
     <t>one_node_small</t>
   </si>
   <si>
-    <t>ferrite</t>
+    <t>ferrite_n20</t>
   </si>
   <si>
     <t>PH</t>
@@ -52,7 +52,7 @@
     <t>1441;2744;3198</t>
   </si>
   <si>
-    <t>0.1;1;100</t>
+    <t>0p1</t>
   </si>
   <si>
     <t>LinearRegression</t>
@@ -67,7 +67,7 @@
     <t/>
   </si>
   <si>
-    <t>martensite</t>
+    <t>ferrite_n100</t>
   </si>
   <si>
     <t>DB</t>
@@ -489,7 +489,7 @@
     <col min="3" max="3" style="13" width="18.433571428571426" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="14" width="17.290714285714284" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="14" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="38.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="20.719285714285714" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="14" width="17.433571428571426" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="14" width="18.719285714285714" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>

</xml_diff>

<commit_message>
update stage 1 targetCurve
</commit_message>
<xml_diff>
--- a/configs/global_config.xlsx
+++ b/configs/global_config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>SLURM_iteration</t>
   </si>
@@ -40,37 +40,37 @@
     <t>optimizerName</t>
   </si>
   <si>
-    <t>deviationPercent</t>
+    <t>deviationPercentX</t>
+  </si>
+  <si>
+    <t>deviationPercentY</t>
   </si>
   <si>
     <t>one_node_small</t>
   </si>
   <si>
+    <t>ferrite_n100</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>1441;2744;3198</t>
+  </si>
+  <si>
+    <t>0p1;1;100</t>
+  </si>
+  <si>
+    <t>LinearRegression</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>one_node_test</t>
+  </si>
+  <si>
     <t>ferrite_n20</t>
-  </si>
-  <si>
-    <t>PH</t>
-  </si>
-  <si>
-    <t>1441;2744;3198</t>
-  </si>
-  <si>
-    <t>0p1</t>
-  </si>
-  <si>
-    <t>LinearRegression</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>one_node_test</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>ferrite_n100</t>
   </si>
   <si>
     <t>DB</t>
@@ -158,11 +158,8 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -178,6 +175,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,18 +487,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="14" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="14" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="13" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="17.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="20.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="13" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="13" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="14" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33" customFormat="1" s="1">
@@ -517,7 +517,7 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -526,16 +526,18 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4"/>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="6">
         <v>30</v>
@@ -544,24 +546,26 @@
         <v>10000</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="F2" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="G2" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="6">
         <v>3</v>
       </c>
-      <c r="J2" s="7"/>
+      <c r="J2" s="6">
+        <v>3</v>
+      </c>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
     </row>
@@ -574,57 +578,49 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="I3" s="8"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F4" s="7"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="5"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="8"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="F5" s="7"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="5"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="8"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
@@ -640,7 +636,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="5"/>
+      <c r="I6" s="8"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -654,7 +650,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="5"/>
+      <c r="I7" s="8"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -663,14 +659,14 @@
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="5"/>
+      <c r="I8" s="8"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -679,14 +675,14 @@
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="5"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="8"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -695,154 +691,154 @@
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="5"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="8"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="5"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="5"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="8"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="5"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="5"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="8"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="5"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="5"/>
+      <c r="I13" s="8"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="5"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="5"/>
+      <c r="I14" s="8"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="5"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="5"/>
+      <c r="I15" s="8"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="5"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="5"/>
+      <c r="I16" s="8"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="5"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="5"/>
+      <c r="I17" s="8"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="5"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="5"/>
+      <c r="I18" s="8"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="5"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
-      <c r="I19" s="5"/>
+      <c r="I19" s="8"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="5"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="5"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="8"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>

</xml_diff>